<commit_message>
Update admin_welcome training form to shrink images and tighten up copy text.
</commit_message>
<xml_diff>
--- a/config/default/forms/training/admin_welcome.xlsx
+++ b/config/default/forms/training/admin_welcome.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -200,13 +200,13 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">label::English (en)</t>
+    <t xml:space="preserve">label::en</t>
   </si>
   <si>
     <t xml:space="preserve">appearance</t>
   </si>
   <si>
-    <t xml:space="preserve">image::English (en)</t>
+    <t xml:space="preserve">image::en</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">welcome</t>
   </si>
   <si>
-    <t xml:space="preserve">Welcome to your new CHT instance! </t>
+    <t xml:space="preserve">NO_LABEL</t>
   </si>
   <si>
     <t xml:space="preserve">field-list</t>
@@ -236,6 +236,27 @@
     <t xml:space="preserve">instance_info</t>
   </si>
   <si>
+    <t xml:space="preserve">Welcome to your new CHT instance! It is running the [Maternal and Newborn Health app](https://docs.communityhealthtoolkit.org/reference-apps/maternal-newborn/).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To configure this instance for your specific workflows, see [the documentation](https://docs.communityhealthtoolkit.org/building/).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household-profile.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add_contacts</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -243,7 +264,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">This instance is currently configured with the default [Maternal and Newborn Health app](</t>
+      <t xml:space="preserve">Get started by [adding contacts and users](</t>
     </r>
     <r>
       <rPr>
@@ -253,7 +274,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">https://docs.communityhealthtoolkit.org/reference-apps/maternal-newborn/</t>
+      <t xml:space="preserve">https://docs.communityhealthtoolkit.org/building/contact-management/contact-and-users-1/</t>
     </r>
     <r>
       <rPr>
@@ -266,40 +287,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">docs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See [the documentation](https://docs.communityhealthtoolkit.org/building/) for details on how to customize the CHT configuration for your specific workflows.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contacts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Contacts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household-profile.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data in the Community Health Toolkit is associated with [contacts](https://docs.communityhealthtoolkit.org/building/contact-management/contacts/) (persons and places).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_contacts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start using this instance by [adding some contacts and then creating a new user](https://docs.communityhealthtoolkit.org/building/contact-management/contact-and-users-1/).</t>
-  </si>
-  <si>
     <t xml:space="preserve">community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The CHT Community</t>
   </si>
   <si>
     <t xml:space="preserve">logo.png</t>
@@ -308,13 +296,13 @@
     <t xml:space="preserve">intro</t>
   </si>
   <si>
-    <t xml:space="preserve">The Community Health Toolkit is maintained by a thriving community of people around the world!</t>
+    <t xml:space="preserve">The CHT is maintained by a community of people around the world.</t>
   </si>
   <si>
     <t xml:space="preserve">forum</t>
   </si>
   <si>
-    <t xml:space="preserve">Please introduce yourself on the [CHT Forum](https://forum.communityhealthtoolkit.org)! This is a great place to find answers to your questions and connect with others who are deploying, configuring, and/or developing software in the CHT ecosystem.</t>
+    <t xml:space="preserve">Introduce yourself on the [CHT Forum](https://forum.communityhealthtoolkit.org)! This is a great place to find answers and connect with others in the community.</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -537,7 +525,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -555,10 +543,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -839,14 +823,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1019"/>
+  <dimension ref="A1:F1018"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -968,7 +952,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
@@ -988,7 +972,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -997,63 +981,65 @@
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>9</v>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>23</v>
       </c>
-      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1061,15 +1047,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1077,10 +1061,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1088,25 +1072,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -9104,88 +9082,31 @@
       <c r="E1018" s="4"/>
       <c r="F1018" s="4"/>
     </row>
-    <row r="1019" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1019" s="4"/>
-      <c r="B1019" s="4"/>
-      <c r="C1019" s="4"/>
-      <c r="D1019" s="4"/>
-      <c r="E1019" s="4"/>
-      <c r="F1019" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:F10 A12:F9996 A11:B11 D11:F11">
+  <conditionalFormatting sqref="A2:F9995">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A3="begin_group"</formula>
+      <formula>$A2="begin_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A3="end_group"</formula>
+      <formula>$A2="end_group"</formula>
     </cfRule>
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A3="begin_repeat"</formula>
+      <formula>$A2="begin_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A3="end_repeat"</formula>
+      <formula>$A2="end_repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A3), NOT(ISBLANK(A3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B9996">
-    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(B3), NOT(ISBLANK($A3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C9996 C3:C10">
-    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C3),NOT(OR(ISBLANK($A3),$A3="calculate")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A11="begin_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A11="end_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A11="begin_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A11="end_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK($A11), NOT(ISBLANK(C11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(ISBLANK(C11),NOT(OR(ISBLANK($A11),$A11="calculate")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>$A2="begin_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>$A2="end_group"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>$A2="begin_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>$A2="end_repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK($A2), NOT(ISBLANK(A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+  <conditionalFormatting sqref="B2:B9995">
+    <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(B2), NOT(ISBLANK($A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+  <conditionalFormatting sqref="C2:C9995">
+    <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(ISBLANK(C2),NOT(OR(ISBLANK($A2),$A2="calculate")))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9194,13 +9115,13 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1011" type="list">
+    <dataValidation allowBlank="true" error="If configuring a select, ensure your list name matches a list from the choices sheet." errorStyle="information" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A1010" type="list">
       <formula1>"begin_group,end_group,note,calculate,text,integer,decimal,select_one list_name,select_multiple list_name,date,time,datetime,begin_repeat,end_repeat,geopoint,geotrace,geoshape,start-geopoint,range,image,audio,video,file,rank,acknowledge,start,end,today"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId2" display="https://docs.communityhealthtoolkit.org/reference-apps/maternal-newborn/"/>
+    <hyperlink ref="C11" r:id="rId2" display="https://docs.communityhealthtoolkit.org/building/contact-management/contact-and-users-1/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -9226,45 +9147,45 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="32.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="20.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="32.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="C2" s="8" t="str">
+        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
+        <v>20250926152620</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="9" t="str">
-        <f aca="true">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20250910160444</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>